<commit_message>
attempt to fix tests
</commit_message>
<xml_diff>
--- a/components/sponsored_benefits/spec/test_data/census_employee_import/DCHL Employee Census.xlsx
+++ b/components/sponsored_benefits/spec/test_data/census_employee_import/DCHL Employee Census.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahulgudi/Documents/ideacrew/enroll/components/sponsored_benefits/spec/test_data/census_employee_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7A21BB-BD9A-C04F-BD37-F487C8B2E68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E300CFC-7279-A44F-A35C-947559CD02E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="14180" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1408,9 +1408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U12" sqref="U12"/>
+      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1640,7 +1640,7 @@
         <v>23445</v>
       </c>
       <c r="V4" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>